<commit_message>
Update Use Case Scenario , sistem Tombole
</commit_message>
<xml_diff>
--- a/UseCase-Scenarij/Scenarij 2 - Servis tombole.xlsx
+++ b/UseCase-Scenarij/Scenarij 2 - Servis tombole.xlsx
@@ -72,10 +72,10 @@
     <t>Osobe koje su se prijavile za vizu i čije prijavnice su u opticaju da budu odabrane.</t>
   </si>
   <si>
-    <t>Nakon isteka roka prijava, usposlenik će iskoristiti sistem za zatvaranje dalje mogućnosti prijave za taj rok. Nakon toga će administrator sistema pokrenuti tombolu koja koristeći svoje sisteme odabira će odabrati primljene/odbijene vize.</t>
-  </si>
-  <si>
     <t>Zbog sigurnosnih koraka koji su prije upotrebe ovog servisa poduzeti alternativnih koraka i proširenja za ovaj konkretan servis nema. Također, sam sistem tombole je rigorozno određen procedurom koja ne smije biti komprimirana od strane alternativnih koraka i korištenja.</t>
+  </si>
+  <si>
+    <t>Nakon isteka roka prijava, automatski će se aktivirati sistem za zatvaranje dalje mogućnosti prijave za taj rok. Nakon toga će administrator sistema pokrenuti tombolu koja koristeći svoje sisteme odabira će odabrati primljene/odbijene vize.</t>
   </si>
 </sst>
 </file>
@@ -565,7 +565,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -584,7 +584,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="47.55" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="63.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -592,7 +592,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="48.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="60.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -600,7 +600,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="58.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="63.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -640,20 +640,20 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="76.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="87.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="97.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="25.85" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>